<commit_message>
Transição incompleta para Excel
Falta tratar o vetor b
</commit_message>
<xml_diff>
--- a/planilha.xlsx
+++ b/planilha.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22313"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A48DA5F1-7DA4-4B5E-9B2B-84B3F31DF038}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{52DAFD66-D254-43A2-9532-A7DE764B71BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -369,96 +369,111 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C1">
+        <v>-1</v>
+      </c>
+      <c r="D1">
+        <v>0</v>
+      </c>
+      <c r="E1">
+        <v>0</v>
+      </c>
+      <c r="F1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>-1</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>-1</v>
+      </c>
+      <c r="D2">
+        <v>-1</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
         <v>2</v>
       </c>
-      <c r="D1">
-        <v>3</v>
-      </c>
-      <c r="E1">
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>-1</v>
+      </c>
+      <c r="B3">
+        <v>-1</v>
+      </c>
+      <c r="C3">
         <v>4</v>
       </c>
+      <c r="D3">
+        <v>-1</v>
+      </c>
+      <c r="E3">
+        <v>-1</v>
+      </c>
+      <c r="F3">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>-1</v>
+      </c>
+      <c r="C4">
+        <v>-1</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>-1</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Transição para Excel completa
Métodos de Elim. Gauss e Seidel feitos
</commit_message>
<xml_diff>
--- a/planilha.xlsx
+++ b/planilha.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22313"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{52DAFD66-D254-43A2-9532-A7DE764B71BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC69EDD1-9E92-4945-ACA5-9DFA34772F94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -369,112 +369,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:4">
       <c r="A1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>-3</v>
+      </c>
+      <c r="D1">
         <v>-1</v>
       </c>
-      <c r="C1">
-        <v>-1</v>
-      </c>
-      <c r="D1">
-        <v>0</v>
-      </c>
-      <c r="E1">
-        <v>0</v>
-      </c>
-      <c r="F1">
-        <v>-1</v>
-      </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>-1</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>-1</v>
-      </c>
-      <c r="E2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>-3</v>
+      </c>
+      <c r="D3">
         <v>0</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3">
-        <v>-1</v>
-      </c>
-      <c r="B3">
-        <v>-1</v>
-      </c>
-      <c r="C3">
-        <v>4</v>
-      </c>
-      <c r="D3">
-        <v>-1</v>
-      </c>
-      <c r="E3">
-        <v>-1</v>
-      </c>
-      <c r="F3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4">
-        <v>0</v>
-      </c>
-      <c r="B4">
-        <v>-1</v>
-      </c>
-      <c r="C4">
-        <v>-1</v>
-      </c>
-      <c r="D4">
-        <v>4</v>
-      </c>
-      <c r="E4">
-        <v>-1</v>
-      </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5">
-        <v>0</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>-1</v>
-      </c>
-      <c r="D5">
-        <v>-1</v>
-      </c>
-      <c r="E5">
-        <v>4</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add autovalor, subs_prim e subs_seg
Função de autovalores
Função subst. primeiro dígito
Função subst. segundo dígito
</commit_message>
<xml_diff>
--- a/planilha.xlsx
+++ b/planilha.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22313"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{52DAFD66-D254-43A2-9532-A7DE764B71BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B53EFF71-CF1E-4E50-8C4B-89BD9E0DCCFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -369,111 +369,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:3">
       <c r="A1">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="B1">
-        <v>-1</v>
+        <v>22</v>
       </c>
       <c r="C1">
-        <v>-1</v>
-      </c>
-      <c r="D1">
-        <v>0</v>
-      </c>
-      <c r="E1">
-        <v>0</v>
-      </c>
-      <c r="F1">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:3">
       <c r="A2">
-        <v>-1</v>
+        <v>48</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C2">
-        <v>-1</v>
-      </c>
-      <c r="D2">
-        <v>-1</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3">
-        <v>-1</v>
-      </c>
-      <c r="B3">
-        <v>-1</v>
-      </c>
-      <c r="C3">
-        <v>4</v>
-      </c>
-      <c r="D3">
-        <v>-1</v>
-      </c>
-      <c r="E3">
-        <v>-1</v>
-      </c>
-      <c r="F3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4">
-        <v>0</v>
-      </c>
-      <c r="B4">
-        <v>-1</v>
-      </c>
-      <c r="C4">
-        <v>-1</v>
-      </c>
-      <c r="D4">
-        <v>4</v>
-      </c>
-      <c r="E4">
-        <v>-1</v>
-      </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5">
-        <v>0</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>-1</v>
-      </c>
-      <c r="D5">
-        <v>-1</v>
-      </c>
-      <c r="E5">
-        <v>4</v>
-      </c>
-      <c r="F5">
         <v>1</v>
       </c>
     </row>

</xml_diff>